<commit_message>
create use and studnetid
</commit_message>
<xml_diff>
--- a/public/studentdata.xlsx
+++ b/public/studentdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="504">
   <si>
     <t>Id</t>
   </si>
@@ -74,6 +74,99 @@
     <t>remark</t>
   </si>
   <si>
+    <t>callstatus</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>bachelor</t>
+  </si>
+  <si>
+    <t>plus2</t>
+  </si>
+  <si>
+    <t>slc</t>
+  </si>
+  <si>
+    <t>major_subject</t>
+  </si>
+  <si>
+    <t>marital_status</t>
+  </si>
+  <si>
+    <t>ielts</t>
+  </si>
+  <si>
+    <t>ielts_ukvi</t>
+  </si>
+  <si>
+    <t>tofel</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>pte</t>
+  </si>
+  <si>
+    <t>gre</t>
+  </si>
+  <si>
+    <t>extra</t>
+  </si>
+  <si>
+    <t>counseled by</t>
+  </si>
+  <si>
+    <t>studentid</t>
+  </si>
+  <si>
+    <t>master_score</t>
+  </si>
+  <si>
+    <t>bachelor_score</t>
+  </si>
+  <si>
+    <t>plus2_score</t>
+  </si>
+  <si>
+    <t>slc_score</t>
+  </si>
+  <si>
+    <t>master_passoutyear</t>
+  </si>
+  <si>
+    <t>bachelor_passoutyear</t>
+  </si>
+  <si>
+    <t>plus2_passoutyear</t>
+  </si>
+  <si>
+    <t>slc_passoutyear</t>
+  </si>
+  <si>
+    <t>ielts_notlessthen</t>
+  </si>
+  <si>
+    <t>ielts_ukvi_notlessthen</t>
+  </si>
+  <si>
+    <t>tofel_notlessthen</t>
+  </si>
+  <si>
+    <t>sat_notlessthen</t>
+  </si>
+  <si>
+    <t>pte_notlessthen</t>
+  </si>
+  <si>
+    <t>gre_notlessthen</t>
+  </si>
+  <si>
     <t>sdads</t>
   </si>
   <si>
@@ -95,6 +188,9 @@
     <t>2023-08-01 12:24:34</t>
   </si>
   <si>
+    <t>called</t>
+  </si>
+  <si>
     <t>2023-08-01 12:28:14</t>
   </si>
   <si>
@@ -1212,6 +1308,225 @@
   </si>
   <si>
     <t>lj</t>
+  </si>
+  <si>
+    <t>Rajan</t>
+  </si>
+  <si>
+    <t>balkumari</t>
+  </si>
+  <si>
+    <t>2 year</t>
+  </si>
+  <si>
+    <t>rajan@gmil.com</t>
+  </si>
+  <si>
+    <t>2023-08-11 11:41:34</t>
+  </si>
+  <si>
+    <t>processing</t>
+  </si>
+  <si>
+    <t>not_called</t>
+  </si>
+  <si>
+    <t>1992-01-01</t>
+  </si>
+  <si>
+    <t>grade :5&amp; passout year :</t>
+  </si>
+  <si>
+    <t>grade :6&amp; passout year :</t>
+  </si>
+  <si>
+    <t>grade :7&amp; passout year :</t>
+  </si>
+  <si>
+    <t>married</t>
+  </si>
+  <si>
+    <t>overall score :7&amp; not less then :6</t>
+  </si>
+  <si>
+    <t>overall score :7&amp; not less then :7</t>
+  </si>
+  <si>
+    <t>overall score :&amp; not less then :7</t>
+  </si>
+  <si>
+    <t>overall score :7&amp; not less then :77</t>
+  </si>
+  <si>
+    <t>radhe</t>
+  </si>
+  <si>
+    <t>2023-08-11 11:47:53</t>
+  </si>
+  <si>
+    <t>1998-01-01</t>
+  </si>
+  <si>
+    <t>grade :&amp; passout year :</t>
+  </si>
+  <si>
+    <t>overall score :&amp; not less then :</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>sajilovisa@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-08-11 12:04:21</t>
+  </si>
+  <si>
+    <t>2023-08-11 12:09:03</t>
+  </si>
+  <si>
+    <t>2022-01-01</t>
+  </si>
+  <si>
+    <t>grade :5&amp; passout year :55</t>
+  </si>
+  <si>
+    <t>grade :6&amp; passout year :66</t>
+  </si>
+  <si>
+    <t>grade :7&amp; passout year :2077</t>
+  </si>
+  <si>
+    <t>grade :7&amp; passout year :7</t>
+  </si>
+  <si>
+    <t>kjk</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>sir</t>
+  </si>
+  <si>
+    <t>didi</t>
+  </si>
+  <si>
+    <t>i have worked in a very prestigious collae of the centurey to gan m educaion that has made all the difference in the work field of he company</t>
+  </si>
+  <si>
+    <t>i have not applied befoe to get any visa rehjetion and i am sure that i will not be any objected t any if he visa eoval rocess the</t>
+  </si>
+  <si>
+    <t>didi@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-08-13 04:52:22</t>
+  </si>
+  <si>
+    <t>2023-08-13 06:47:04</t>
+  </si>
+  <si>
+    <t>divorced</t>
+  </si>
+  <si>
+    <t>overall score :67&amp; not less then :67</t>
+  </si>
+  <si>
+    <t>raju sir</t>
+  </si>
+  <si>
+    <t>master in software engineering</t>
+  </si>
+  <si>
+    <t>bachelor in software engineering</t>
+  </si>
+  <si>
+    <t>naruto</t>
+  </si>
+  <si>
+    <t>hidden leaf village</t>
+  </si>
+  <si>
+    <t>a+</t>
+  </si>
+  <si>
+    <t>japan</t>
+  </si>
+  <si>
+    <t>technology</t>
+  </si>
+  <si>
+    <t>3 year of experience</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>naruto@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-08-13 05:52:21</t>
+  </si>
+  <si>
+    <t>2023-08-14 05:12:20</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>1998-09-01</t>
+  </si>
+  <si>
+    <t>master in science and echnology</t>
+  </si>
+  <si>
+    <t>science and technology</t>
+  </si>
+  <si>
+    <t>anushil</t>
+  </si>
+  <si>
+    <t>79%</t>
+  </si>
+  <si>
+    <t>Anushil</t>
+  </si>
+  <si>
+    <t>kausahlatar</t>
+  </si>
+  <si>
+    <t>anu@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-08-14 05:50:53</t>
+  </si>
+  <si>
+    <t>2021-03-09</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>2023-08-14 06:59:56</t>
+  </si>
+  <si>
+    <t>sv-02383</t>
+  </si>
+  <si>
+    <t>2023-08-14 07:03:23</t>
+  </si>
+  <si>
+    <t>sv-02384</t>
+  </si>
+  <si>
+    <t>anushilkarki@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-08-14 07:03:45</t>
+  </si>
+  <si>
+    <t>sv-02385</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1866,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:AX51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1559,7 +1874,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:50">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1617,579 +1932,659 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2"/>
+        <v>51</v>
+      </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2"/>
-      <c r="O2"/>
+        <v>51</v>
+      </c>
       <c r="P2" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2"/>
-      <c r="S2"/>
-    </row>
-    <row r="3" spans="1:19">
+        <v>56</v>
+      </c>
+      <c r="T2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3"/>
+        <v>51</v>
+      </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3"/>
-      <c r="O3"/>
+        <v>51</v>
+      </c>
       <c r="P3" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3"/>
-      <c r="S3"/>
-    </row>
-    <row r="4" spans="1:19">
+        <v>58</v>
+      </c>
+      <c r="T3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="M4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4"/>
-      <c r="O4"/>
+        <v>70</v>
+      </c>
       <c r="P4" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="Q4" t="s">
-        <v>39</v>
-      </c>
-      <c r="R4"/>
-      <c r="S4"/>
-    </row>
-    <row r="5" spans="1:19">
+        <v>71</v>
+      </c>
+      <c r="T4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="M5" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5"/>
-      <c r="O5"/>
+        <v>83</v>
+      </c>
       <c r="P5" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="Q5" t="s">
-        <v>39</v>
-      </c>
-      <c r="R5"/>
-      <c r="S5"/>
-    </row>
-    <row r="6" spans="1:19">
+        <v>71</v>
+      </c>
+      <c r="T5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="G6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" t="s">
+        <v>93</v>
+      </c>
+      <c r="L6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M6" t="s">
+        <v>95</v>
+      </c>
+      <c r="P6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T6" t="s">
         <v>57</v>
       </c>
-      <c r="H6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M6" t="s">
-        <v>63</v>
-      </c>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>39</v>
-      </c>
-      <c r="R6"/>
-      <c r="S6"/>
-    </row>
-    <row r="7" spans="1:19">
+    </row>
+    <row r="7" spans="1:50">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" t="s">
+        <v>107</v>
+      </c>
+      <c r="P7" t="s">
         <v>71</v>
       </c>
-      <c r="J7" t="s">
-        <v>72</v>
-      </c>
-      <c r="K7" t="s">
-        <v>73</v>
-      </c>
-      <c r="L7" t="s">
-        <v>74</v>
-      </c>
-      <c r="M7" t="s">
-        <v>75</v>
-      </c>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7" t="s">
-        <v>39</v>
-      </c>
       <c r="Q7" t="s">
-        <v>39</v>
-      </c>
-      <c r="R7"/>
-      <c r="S7"/>
-    </row>
-    <row r="8" spans="1:19">
+        <v>71</v>
+      </c>
+      <c r="T7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="J8" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="L8" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="M8" t="s">
-        <v>87</v>
-      </c>
-      <c r="N8"/>
-      <c r="O8"/>
+        <v>119</v>
+      </c>
       <c r="P8" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="Q8" t="s">
-        <v>39</v>
-      </c>
-      <c r="R8"/>
-      <c r="S8"/>
-    </row>
-    <row r="9" spans="1:19">
+        <v>71</v>
+      </c>
+      <c r="T8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50">
       <c r="A9">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="G9" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="H9" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="I9" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="J9" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="K9" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="L9" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="M9" t="s">
-        <v>99</v>
-      </c>
-      <c r="N9"/>
-      <c r="O9"/>
+        <v>131</v>
+      </c>
       <c r="P9" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="Q9" t="s">
-        <v>39</v>
-      </c>
-      <c r="R9"/>
-      <c r="S9"/>
-    </row>
-    <row r="10" spans="1:19">
+        <v>71</v>
+      </c>
+      <c r="T9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50">
       <c r="A10">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="G10" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="H10" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="I10" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="J10" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="K10" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="L10" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="M10" t="s">
-        <v>111</v>
-      </c>
-      <c r="N10"/>
-      <c r="O10"/>
+        <v>143</v>
+      </c>
       <c r="P10" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="Q10" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10"/>
-      <c r="S10"/>
-    </row>
-    <row r="11" spans="1:19">
+        <v>71</v>
+      </c>
+      <c r="T10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50">
       <c r="A11">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="H11" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="I11" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="J11" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="K11" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="L11" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="M11" t="s">
-        <v>123</v>
-      </c>
-      <c r="N11"/>
-      <c r="O11"/>
+        <v>155</v>
+      </c>
       <c r="P11" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="Q11" t="s">
-        <v>39</v>
-      </c>
-      <c r="R11"/>
-      <c r="S11"/>
-    </row>
-    <row r="12" spans="1:19">
+        <v>71</v>
+      </c>
+      <c r="T11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50">
       <c r="A12">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="E12" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="F12" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="H12" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="I12" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="J12" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="K12" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="L12" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="M12" t="s">
-        <v>135</v>
-      </c>
-      <c r="N12"/>
-      <c r="O12"/>
+        <v>167</v>
+      </c>
       <c r="P12" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="Q12" t="s">
-        <v>39</v>
-      </c>
-      <c r="R12"/>
-      <c r="S12"/>
-    </row>
-    <row r="13" spans="1:19">
+        <v>71</v>
+      </c>
+      <c r="T12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50">
       <c r="A13">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C13">
         <v>9843777683</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F13">
         <v>2.592</v>
@@ -2201,503 +2596,492 @@
         <v>7</v>
       </c>
       <c r="I13" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J13" t="s">
-        <v>140</v>
-      </c>
-      <c r="K13"/>
+        <v>172</v>
+      </c>
       <c r="L13" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M13" t="s">
-        <v>142</v>
-      </c>
-      <c r="N13"/>
-      <c r="O13"/>
+        <v>174</v>
+      </c>
       <c r="P13" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="Q13" t="s">
-        <v>143</v>
-      </c>
-      <c r="R13"/>
-      <c r="S13"/>
-    </row>
-    <row r="14" spans="1:19">
+        <v>175</v>
+      </c>
+      <c r="T13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50">
       <c r="A14">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
       <c r="F14" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="G14" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="H14" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="I14" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="J14" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
       <c r="K14" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="L14" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="M14" t="s">
-        <v>155</v>
-      </c>
-      <c r="N14"/>
-      <c r="O14"/>
+        <v>187</v>
+      </c>
       <c r="P14" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="Q14" t="s">
-        <v>156</v>
-      </c>
-      <c r="R14"/>
-      <c r="S14"/>
-    </row>
-    <row r="15" spans="1:19">
+        <v>188</v>
+      </c>
+      <c r="T14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50">
       <c r="A15">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="C15" t="s">
-        <v>158</v>
+        <v>190</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>191</v>
       </c>
       <c r="E15" t="s">
-        <v>160</v>
+        <v>192</v>
       </c>
       <c r="F15" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="G15" t="s">
-        <v>162</v>
+        <v>194</v>
       </c>
       <c r="H15" t="s">
-        <v>163</v>
+        <v>195</v>
       </c>
       <c r="I15" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="J15" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
       <c r="K15" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="L15" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
       <c r="M15" t="s">
-        <v>168</v>
-      </c>
-      <c r="N15"/>
-      <c r="O15"/>
+        <v>200</v>
+      </c>
       <c r="P15" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="Q15" t="s">
-        <v>156</v>
-      </c>
-      <c r="R15"/>
-      <c r="S15"/>
-    </row>
-    <row r="16" spans="1:19">
+        <v>188</v>
+      </c>
+      <c r="T15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50">
       <c r="A16">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>201</v>
       </c>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>202</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
       <c r="E16" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="F16" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
       <c r="G16" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="H16" t="s">
-        <v>175</v>
+        <v>207</v>
       </c>
       <c r="I16" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="J16" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="K16" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="L16" t="s">
-        <v>179</v>
+        <v>211</v>
       </c>
       <c r="M16" t="s">
-        <v>180</v>
-      </c>
-      <c r="N16"/>
-      <c r="O16"/>
+        <v>212</v>
+      </c>
       <c r="P16" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="Q16" t="s">
-        <v>156</v>
-      </c>
-      <c r="R16"/>
-      <c r="S16"/>
-    </row>
-    <row r="17" spans="1:19">
+        <v>188</v>
+      </c>
+      <c r="T16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:50">
       <c r="A17">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="E17" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="F17" t="s">
-        <v>185</v>
+        <v>217</v>
       </c>
       <c r="G17" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="H17" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="I17" t="s">
+        <v>220</v>
+      </c>
+      <c r="J17" t="s">
+        <v>221</v>
+      </c>
+      <c r="K17" t="s">
+        <v>222</v>
+      </c>
+      <c r="L17" t="s">
+        <v>223</v>
+      </c>
+      <c r="M17" t="s">
+        <v>224</v>
+      </c>
+      <c r="P17" t="s">
         <v>188</v>
       </c>
-      <c r="J17" t="s">
-        <v>189</v>
-      </c>
-      <c r="K17" t="s">
-        <v>190</v>
-      </c>
-      <c r="L17" t="s">
-        <v>191</v>
-      </c>
-      <c r="M17" t="s">
-        <v>192</v>
-      </c>
-      <c r="N17"/>
-      <c r="O17"/>
-      <c r="P17" t="s">
-        <v>156</v>
-      </c>
       <c r="Q17" t="s">
-        <v>156</v>
-      </c>
-      <c r="R17"/>
-      <c r="S17"/>
-    </row>
-    <row r="18" spans="1:19">
+        <v>188</v>
+      </c>
+      <c r="T17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:50">
       <c r="A18">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="D18" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="E18" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
       <c r="F18" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="G18" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="H18" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="I18" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="J18" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
       <c r="K18" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="L18" t="s">
-        <v>203</v>
+        <v>235</v>
       </c>
       <c r="M18" t="s">
-        <v>204</v>
-      </c>
-      <c r="N18"/>
-      <c r="O18"/>
+        <v>236</v>
+      </c>
       <c r="P18" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="Q18" t="s">
-        <v>156</v>
-      </c>
-      <c r="R18"/>
-      <c r="S18"/>
-    </row>
-    <row r="19" spans="1:19">
+        <v>188</v>
+      </c>
+      <c r="T18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:50">
       <c r="A19">
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
       <c r="C19" t="s">
-        <v>206</v>
+        <v>238</v>
       </c>
       <c r="D19" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
       <c r="E19" t="s">
-        <v>208</v>
+        <v>240</v>
       </c>
       <c r="F19" t="s">
-        <v>209</v>
+        <v>241</v>
       </c>
       <c r="G19" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="H19" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
       <c r="I19" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
       <c r="J19" t="s">
-        <v>213</v>
+        <v>245</v>
       </c>
       <c r="K19" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="L19" t="s">
-        <v>215</v>
+        <v>247</v>
       </c>
       <c r="M19" t="s">
-        <v>216</v>
-      </c>
-      <c r="N19"/>
-      <c r="O19"/>
+        <v>248</v>
+      </c>
       <c r="P19" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="Q19" t="s">
-        <v>156</v>
-      </c>
-      <c r="R19"/>
-      <c r="S19"/>
-    </row>
-    <row r="20" spans="1:19">
+        <v>188</v>
+      </c>
+      <c r="T19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:50">
       <c r="A20">
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>217</v>
+        <v>249</v>
       </c>
       <c r="C20" t="s">
-        <v>218</v>
+        <v>250</v>
       </c>
       <c r="D20" t="s">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="E20" t="s">
-        <v>220</v>
+        <v>252</v>
       </c>
       <c r="F20" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
       <c r="G20" t="s">
-        <v>222</v>
+        <v>254</v>
       </c>
       <c r="H20" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="I20" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="J20" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
       <c r="K20" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
       <c r="L20" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="M20" t="s">
-        <v>228</v>
-      </c>
-      <c r="N20"/>
-      <c r="O20"/>
+        <v>260</v>
+      </c>
       <c r="P20" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="Q20" t="s">
-        <v>156</v>
-      </c>
-      <c r="R20"/>
-      <c r="S20"/>
-    </row>
-    <row r="21" spans="1:19">
+        <v>188</v>
+      </c>
+      <c r="T20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:50">
       <c r="A21">
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="C21" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="D21" t="s">
-        <v>231</v>
+        <v>263</v>
       </c>
       <c r="E21" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="F21" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="G21" t="s">
-        <v>234</v>
+        <v>266</v>
       </c>
       <c r="H21" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="I21" t="s">
-        <v>236</v>
+        <v>268</v>
       </c>
       <c r="J21" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="K21" t="s">
-        <v>238</v>
+        <v>270</v>
       </c>
       <c r="L21" t="s">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="M21" t="s">
-        <v>240</v>
-      </c>
-      <c r="N21"/>
-      <c r="O21"/>
+        <v>272</v>
+      </c>
       <c r="P21" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="Q21" t="s">
-        <v>156</v>
-      </c>
-      <c r="R21"/>
-      <c r="S21"/>
-    </row>
-    <row r="22" spans="1:19">
+        <v>188</v>
+      </c>
+      <c r="T21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:50">
       <c r="A22">
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>241</v>
+        <v>273</v>
       </c>
       <c r="C22" t="s">
-        <v>242</v>
+        <v>274</v>
       </c>
       <c r="D22" t="s">
-        <v>243</v>
+        <v>275</v>
       </c>
       <c r="E22" t="s">
-        <v>244</v>
+        <v>276</v>
       </c>
       <c r="F22" t="s">
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="G22" t="s">
-        <v>246</v>
+        <v>278</v>
       </c>
       <c r="H22" t="s">
-        <v>247</v>
+        <v>279</v>
       </c>
       <c r="I22" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
       <c r="J22" t="s">
-        <v>249</v>
+        <v>281</v>
       </c>
       <c r="K22" t="s">
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="L22" t="s">
-        <v>251</v>
+        <v>283</v>
       </c>
       <c r="M22" t="s">
-        <v>252</v>
-      </c>
-      <c r="N22"/>
-      <c r="O22"/>
+        <v>284</v>
+      </c>
       <c r="P22" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="Q22" t="s">
-        <v>156</v>
-      </c>
-      <c r="R22"/>
-      <c r="S22"/>
-    </row>
-    <row r="23" spans="1:19">
+        <v>188</v>
+      </c>
+      <c r="T22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:50">
       <c r="A23">
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C23">
         <v>9843777683</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F23">
         <v>2.592</v>
@@ -2709,554 +3093,542 @@
         <v>7</v>
       </c>
       <c r="I23" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J23" t="s">
-        <v>140</v>
-      </c>
-      <c r="K23"/>
+        <v>172</v>
+      </c>
       <c r="L23" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M23" t="s">
-        <v>142</v>
-      </c>
-      <c r="N23"/>
-      <c r="O23"/>
+        <v>174</v>
+      </c>
       <c r="P23" t="s">
-        <v>253</v>
+        <v>285</v>
       </c>
       <c r="Q23" t="s">
-        <v>253</v>
-      </c>
-      <c r="R23"/>
-      <c r="S23"/>
-    </row>
-    <row r="24" spans="1:19">
+        <v>285</v>
+      </c>
+      <c r="T23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:50">
       <c r="A24">
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
       <c r="C24" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
       <c r="D24" t="s">
-        <v>256</v>
+        <v>288</v>
       </c>
       <c r="E24" t="s">
-        <v>257</v>
+        <v>289</v>
       </c>
       <c r="F24" t="s">
-        <v>258</v>
+        <v>290</v>
       </c>
       <c r="G24" t="s">
-        <v>259</v>
+        <v>291</v>
       </c>
       <c r="H24" t="s">
-        <v>260</v>
+        <v>292</v>
       </c>
       <c r="I24" t="s">
-        <v>261</v>
+        <v>293</v>
       </c>
       <c r="J24" t="s">
-        <v>262</v>
+        <v>294</v>
       </c>
       <c r="K24" t="s">
-        <v>263</v>
+        <v>295</v>
       </c>
       <c r="L24" t="s">
-        <v>264</v>
+        <v>296</v>
       </c>
       <c r="M24" t="s">
-        <v>265</v>
-      </c>
-      <c r="N24"/>
-      <c r="O24"/>
+        <v>297</v>
+      </c>
       <c r="P24" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="Q24" t="s">
-        <v>266</v>
-      </c>
-      <c r="R24"/>
-      <c r="S24"/>
-    </row>
-    <row r="25" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:50">
       <c r="A25">
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>267</v>
+        <v>299</v>
       </c>
       <c r="C25" t="s">
-        <v>268</v>
+        <v>300</v>
       </c>
       <c r="D25" t="s">
-        <v>269</v>
+        <v>301</v>
       </c>
       <c r="E25" t="s">
-        <v>270</v>
+        <v>302</v>
       </c>
       <c r="F25" t="s">
-        <v>271</v>
+        <v>303</v>
       </c>
       <c r="G25" t="s">
-        <v>272</v>
+        <v>304</v>
       </c>
       <c r="H25" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="I25" t="s">
-        <v>274</v>
+        <v>306</v>
       </c>
       <c r="J25" t="s">
-        <v>275</v>
+        <v>307</v>
       </c>
       <c r="K25" t="s">
-        <v>276</v>
+        <v>308</v>
       </c>
       <c r="L25" t="s">
-        <v>277</v>
+        <v>309</v>
       </c>
       <c r="M25" t="s">
-        <v>278</v>
-      </c>
-      <c r="N25"/>
-      <c r="O25"/>
+        <v>310</v>
+      </c>
       <c r="P25" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="Q25" t="s">
-        <v>266</v>
-      </c>
-      <c r="R25"/>
-      <c r="S25"/>
-    </row>
-    <row r="26" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:50">
       <c r="A26">
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="C26" t="s">
-        <v>280</v>
+        <v>312</v>
       </c>
       <c r="D26" t="s">
-        <v>281</v>
+        <v>313</v>
       </c>
       <c r="E26" t="s">
-        <v>282</v>
+        <v>314</v>
       </c>
       <c r="F26" t="s">
-        <v>283</v>
+        <v>315</v>
       </c>
       <c r="G26" t="s">
-        <v>284</v>
+        <v>316</v>
       </c>
       <c r="H26" t="s">
-        <v>285</v>
+        <v>317</v>
       </c>
       <c r="I26" t="s">
-        <v>286</v>
+        <v>318</v>
       </c>
       <c r="J26" t="s">
-        <v>287</v>
+        <v>319</v>
       </c>
       <c r="K26" t="s">
-        <v>288</v>
+        <v>320</v>
       </c>
       <c r="L26" t="s">
-        <v>289</v>
+        <v>321</v>
       </c>
       <c r="M26" t="s">
-        <v>290</v>
-      </c>
-      <c r="N26"/>
-      <c r="O26"/>
+        <v>322</v>
+      </c>
       <c r="P26" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="Q26" t="s">
-        <v>266</v>
-      </c>
-      <c r="R26"/>
-      <c r="S26"/>
-    </row>
-    <row r="27" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:50">
       <c r="A27">
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>291</v>
+        <v>323</v>
       </c>
       <c r="C27" t="s">
-        <v>292</v>
+        <v>324</v>
       </c>
       <c r="D27" t="s">
-        <v>293</v>
+        <v>325</v>
       </c>
       <c r="E27" t="s">
-        <v>294</v>
+        <v>326</v>
       </c>
       <c r="F27" t="s">
-        <v>295</v>
+        <v>327</v>
       </c>
       <c r="G27" t="s">
-        <v>296</v>
+        <v>328</v>
       </c>
       <c r="H27" t="s">
-        <v>297</v>
+        <v>329</v>
       </c>
       <c r="I27" t="s">
+        <v>330</v>
+      </c>
+      <c r="J27" t="s">
+        <v>331</v>
+      </c>
+      <c r="K27" t="s">
+        <v>332</v>
+      </c>
+      <c r="L27" t="s">
+        <v>333</v>
+      </c>
+      <c r="M27" t="s">
+        <v>334</v>
+      </c>
+      <c r="P27" t="s">
         <v>298</v>
       </c>
-      <c r="J27" t="s">
-        <v>299</v>
-      </c>
-      <c r="K27" t="s">
-        <v>300</v>
-      </c>
-      <c r="L27" t="s">
-        <v>301</v>
-      </c>
-      <c r="M27" t="s">
-        <v>302</v>
-      </c>
-      <c r="N27"/>
-      <c r="O27"/>
-      <c r="P27" t="s">
-        <v>266</v>
-      </c>
       <c r="Q27" t="s">
-        <v>266</v>
-      </c>
-      <c r="R27"/>
-      <c r="S27"/>
-    </row>
-    <row r="28" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:50">
       <c r="A28">
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>303</v>
+        <v>335</v>
       </c>
       <c r="C28" t="s">
-        <v>304</v>
+        <v>336</v>
       </c>
       <c r="D28" t="s">
-        <v>305</v>
+        <v>337</v>
       </c>
       <c r="E28" t="s">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c r="F28" t="s">
-        <v>307</v>
+        <v>339</v>
       </c>
       <c r="G28" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
       <c r="H28" t="s">
-        <v>309</v>
+        <v>341</v>
       </c>
       <c r="I28" t="s">
-        <v>310</v>
+        <v>342</v>
       </c>
       <c r="J28" t="s">
-        <v>311</v>
+        <v>343</v>
       </c>
       <c r="K28" t="s">
-        <v>312</v>
+        <v>344</v>
       </c>
       <c r="L28" t="s">
-        <v>313</v>
+        <v>345</v>
       </c>
       <c r="M28" t="s">
-        <v>314</v>
-      </c>
-      <c r="N28"/>
-      <c r="O28"/>
+        <v>346</v>
+      </c>
       <c r="P28" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="Q28" t="s">
-        <v>266</v>
-      </c>
-      <c r="R28"/>
-      <c r="S28"/>
-    </row>
-    <row r="29" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:50">
       <c r="A29">
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>315</v>
+        <v>347</v>
       </c>
       <c r="C29" t="s">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c r="D29" t="s">
-        <v>317</v>
+        <v>349</v>
       </c>
       <c r="E29" t="s">
-        <v>318</v>
+        <v>350</v>
       </c>
       <c r="F29" t="s">
-        <v>319</v>
+        <v>351</v>
       </c>
       <c r="G29" t="s">
-        <v>320</v>
+        <v>352</v>
       </c>
       <c r="H29" t="s">
-        <v>321</v>
+        <v>353</v>
       </c>
       <c r="I29" t="s">
-        <v>322</v>
+        <v>354</v>
       </c>
       <c r="J29" t="s">
-        <v>323</v>
+        <v>355</v>
       </c>
       <c r="K29" t="s">
-        <v>324</v>
+        <v>356</v>
       </c>
       <c r="L29" t="s">
-        <v>325</v>
+        <v>357</v>
       </c>
       <c r="M29" t="s">
-        <v>326</v>
-      </c>
-      <c r="N29"/>
-      <c r="O29"/>
+        <v>358</v>
+      </c>
       <c r="P29" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="Q29" t="s">
-        <v>266</v>
-      </c>
-      <c r="R29"/>
-      <c r="S29"/>
-    </row>
-    <row r="30" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:50">
       <c r="A30">
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>327</v>
+        <v>359</v>
       </c>
       <c r="C30" t="s">
-        <v>328</v>
+        <v>360</v>
       </c>
       <c r="D30" t="s">
-        <v>329</v>
+        <v>361</v>
       </c>
       <c r="E30" t="s">
-        <v>330</v>
+        <v>362</v>
       </c>
       <c r="F30" t="s">
-        <v>331</v>
+        <v>363</v>
       </c>
       <c r="G30" t="s">
-        <v>332</v>
+        <v>364</v>
       </c>
       <c r="H30" t="s">
-        <v>333</v>
+        <v>365</v>
       </c>
       <c r="I30" t="s">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c r="J30" t="s">
-        <v>335</v>
+        <v>367</v>
       </c>
       <c r="K30" t="s">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c r="L30" t="s">
-        <v>337</v>
+        <v>369</v>
       </c>
       <c r="M30" t="s">
-        <v>338</v>
-      </c>
-      <c r="N30"/>
-      <c r="O30"/>
+        <v>370</v>
+      </c>
       <c r="P30" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="Q30" t="s">
-        <v>266</v>
-      </c>
-      <c r="R30"/>
-      <c r="S30"/>
-    </row>
-    <row r="31" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:50">
       <c r="A31">
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>339</v>
+        <v>371</v>
       </c>
       <c r="C31" t="s">
-        <v>340</v>
+        <v>372</v>
       </c>
       <c r="D31" t="s">
-        <v>341</v>
+        <v>373</v>
       </c>
       <c r="E31" t="s">
-        <v>342</v>
+        <v>374</v>
       </c>
       <c r="F31" t="s">
-        <v>343</v>
+        <v>375</v>
       </c>
       <c r="G31" t="s">
-        <v>344</v>
+        <v>376</v>
       </c>
       <c r="H31" t="s">
-        <v>345</v>
+        <v>377</v>
       </c>
       <c r="I31" t="s">
-        <v>346</v>
+        <v>378</v>
       </c>
       <c r="J31" t="s">
-        <v>347</v>
+        <v>379</v>
       </c>
       <c r="K31" t="s">
-        <v>348</v>
+        <v>380</v>
       </c>
       <c r="L31" t="s">
-        <v>349</v>
+        <v>381</v>
       </c>
       <c r="M31" t="s">
-        <v>350</v>
-      </c>
-      <c r="N31"/>
-      <c r="O31"/>
+        <v>382</v>
+      </c>
       <c r="P31" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="Q31" t="s">
-        <v>266</v>
-      </c>
-      <c r="R31"/>
-      <c r="S31"/>
-    </row>
-    <row r="32" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:50">
       <c r="A32">
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>351</v>
+        <v>383</v>
       </c>
       <c r="C32" t="s">
-        <v>352</v>
+        <v>384</v>
       </c>
       <c r="D32" t="s">
-        <v>353</v>
+        <v>385</v>
       </c>
       <c r="E32" t="s">
-        <v>354</v>
+        <v>386</v>
       </c>
       <c r="F32" t="s">
-        <v>355</v>
+        <v>387</v>
       </c>
       <c r="G32" t="s">
-        <v>356</v>
+        <v>388</v>
       </c>
       <c r="H32" t="s">
-        <v>357</v>
+        <v>389</v>
       </c>
       <c r="I32" t="s">
-        <v>358</v>
+        <v>390</v>
       </c>
       <c r="J32" t="s">
-        <v>359</v>
+        <v>391</v>
       </c>
       <c r="K32" t="s">
-        <v>360</v>
+        <v>392</v>
       </c>
       <c r="L32" t="s">
-        <v>361</v>
+        <v>393</v>
       </c>
       <c r="M32" t="s">
-        <v>362</v>
-      </c>
-      <c r="N32"/>
-      <c r="O32"/>
+        <v>394</v>
+      </c>
       <c r="P32" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="Q32" t="s">
-        <v>266</v>
-      </c>
-      <c r="R32"/>
-      <c r="S32"/>
-    </row>
-    <row r="33" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:50">
       <c r="A33">
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>363</v>
+        <v>395</v>
       </c>
       <c r="C33" t="s">
-        <v>364</v>
+        <v>396</v>
       </c>
       <c r="D33" t="s">
-        <v>365</v>
+        <v>397</v>
       </c>
       <c r="E33" t="s">
-        <v>366</v>
+        <v>398</v>
       </c>
       <c r="F33" t="s">
-        <v>367</v>
+        <v>399</v>
       </c>
       <c r="G33" t="s">
-        <v>368</v>
+        <v>400</v>
       </c>
       <c r="H33" t="s">
-        <v>369</v>
+        <v>401</v>
       </c>
       <c r="I33" t="s">
-        <v>370</v>
+        <v>402</v>
       </c>
       <c r="J33" t="s">
-        <v>371</v>
+        <v>403</v>
       </c>
       <c r="K33" t="s">
-        <v>372</v>
+        <v>404</v>
       </c>
       <c r="L33" t="s">
-        <v>373</v>
+        <v>405</v>
       </c>
       <c r="M33" t="s">
-        <v>374</v>
-      </c>
-      <c r="N33"/>
-      <c r="O33"/>
+        <v>406</v>
+      </c>
       <c r="P33" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="Q33" t="s">
-        <v>266</v>
-      </c>
-      <c r="R33"/>
-      <c r="S33"/>
-    </row>
-    <row r="34" spans="1:19">
+        <v>298</v>
+      </c>
+      <c r="T33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:50">
       <c r="A34">
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C34">
         <v>9843777683</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F34">
         <v>2.592</v>
@@ -3268,44 +3640,42 @@
         <v>7</v>
       </c>
       <c r="I34" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J34" t="s">
-        <v>140</v>
-      </c>
-      <c r="K34"/>
+        <v>172</v>
+      </c>
       <c r="L34" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M34" t="s">
-        <v>142</v>
-      </c>
-      <c r="N34"/>
-      <c r="O34"/>
+        <v>174</v>
+      </c>
       <c r="P34" t="s">
-        <v>375</v>
+        <v>407</v>
       </c>
       <c r="Q34" t="s">
-        <v>375</v>
-      </c>
-      <c r="R34"/>
-      <c r="S34"/>
-    </row>
-    <row r="35" spans="1:19">
+        <v>407</v>
+      </c>
+      <c r="T34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:50">
       <c r="A35">
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C35">
         <v>9843777683</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F35">
         <v>2.592</v>
@@ -3317,44 +3687,42 @@
         <v>7</v>
       </c>
       <c r="I35" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J35" t="s">
-        <v>140</v>
-      </c>
-      <c r="K35"/>
+        <v>172</v>
+      </c>
       <c r="L35" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M35" t="s">
-        <v>142</v>
-      </c>
-      <c r="N35"/>
-      <c r="O35"/>
+        <v>174</v>
+      </c>
       <c r="P35" t="s">
-        <v>376</v>
+        <v>408</v>
       </c>
       <c r="Q35" t="s">
-        <v>376</v>
-      </c>
-      <c r="R35"/>
-      <c r="S35"/>
-    </row>
-    <row r="36" spans="1:19">
+        <v>408</v>
+      </c>
+      <c r="T35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:50">
       <c r="A36">
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C36">
         <v>9843777683</v>
       </c>
       <c r="D36" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F36">
         <v>2.592</v>
@@ -3366,46 +3734,45 @@
         <v>7</v>
       </c>
       <c r="I36" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J36" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="K36" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="L36" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M36" t="s">
-        <v>142</v>
-      </c>
-      <c r="N36"/>
-      <c r="O36"/>
+        <v>174</v>
+      </c>
       <c r="P36" t="s">
-        <v>377</v>
+        <v>409</v>
       </c>
       <c r="Q36" t="s">
-        <v>378</v>
-      </c>
-      <c r="R36"/>
-      <c r="S36"/>
-    </row>
-    <row r="37" spans="1:19">
+        <v>410</v>
+      </c>
+      <c r="T36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:50">
       <c r="A37">
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C37">
         <v>9843777683</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F37">
         <v>2.592</v>
@@ -3417,46 +3784,45 @@
         <v>7</v>
       </c>
       <c r="I37" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J37" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="K37" t="s">
-        <v>379</v>
+        <v>411</v>
       </c>
       <c r="L37" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M37" t="s">
-        <v>142</v>
-      </c>
-      <c r="N37"/>
-      <c r="O37"/>
+        <v>174</v>
+      </c>
       <c r="P37" t="s">
-        <v>380</v>
+        <v>412</v>
       </c>
       <c r="Q37" t="s">
-        <v>381</v>
-      </c>
-      <c r="R37"/>
-      <c r="S37"/>
-    </row>
-    <row r="38" spans="1:19">
+        <v>413</v>
+      </c>
+      <c r="T37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:50">
       <c r="A38">
         <v>66</v>
       </c>
       <c r="B38" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C38">
         <v>9843777683</v>
       </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F38">
         <v>2.592</v>
@@ -3468,46 +3834,45 @@
         <v>7</v>
       </c>
       <c r="I38" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J38" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="K38" t="s">
-        <v>382</v>
+        <v>414</v>
       </c>
       <c r="L38" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M38" t="s">
-        <v>142</v>
-      </c>
-      <c r="N38"/>
-      <c r="O38"/>
+        <v>174</v>
+      </c>
       <c r="P38" t="s">
-        <v>383</v>
+        <v>415</v>
       </c>
       <c r="Q38" t="s">
-        <v>383</v>
-      </c>
-      <c r="R38"/>
-      <c r="S38"/>
-    </row>
-    <row r="39" spans="1:19">
+        <v>415</v>
+      </c>
+      <c r="T38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:50">
       <c r="A39">
         <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C39">
         <v>9843777683</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F39">
         <v>2.592</v>
@@ -3519,46 +3884,45 @@
         <v>7</v>
       </c>
       <c r="I39" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J39" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="K39" t="s">
-        <v>382</v>
+        <v>414</v>
       </c>
       <c r="L39" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M39" t="s">
-        <v>142</v>
-      </c>
-      <c r="N39"/>
-      <c r="O39"/>
+        <v>174</v>
+      </c>
       <c r="P39" t="s">
-        <v>384</v>
+        <v>416</v>
       </c>
       <c r="Q39" t="s">
-        <v>384</v>
-      </c>
-      <c r="R39"/>
-      <c r="S39"/>
-    </row>
-    <row r="40" spans="1:19">
+        <v>416</v>
+      </c>
+      <c r="T39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:50">
       <c r="A40">
         <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C40">
         <v>9843777683</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F40">
         <v>2.592</v>
@@ -3570,46 +3934,45 @@
         <v>7</v>
       </c>
       <c r="I40" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J40" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="K40" t="s">
-        <v>382</v>
+        <v>414</v>
       </c>
       <c r="L40" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M40" t="s">
-        <v>142</v>
-      </c>
-      <c r="N40"/>
-      <c r="O40"/>
+        <v>174</v>
+      </c>
       <c r="P40" t="s">
-        <v>385</v>
+        <v>417</v>
       </c>
       <c r="Q40" t="s">
-        <v>385</v>
-      </c>
-      <c r="R40"/>
-      <c r="S40"/>
-    </row>
-    <row r="41" spans="1:19">
+        <v>417</v>
+      </c>
+      <c r="T40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:50">
       <c r="A41">
         <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C41">
         <v>9843777683</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F41">
         <v>2.592</v>
@@ -3621,88 +3984,816 @@
         <v>7</v>
       </c>
       <c r="I41" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J41" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="K41" t="s">
-        <v>379</v>
+        <v>411</v>
       </c>
       <c r="L41" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="M41" t="s">
-        <v>142</v>
-      </c>
-      <c r="N41"/>
-      <c r="O41"/>
+        <v>174</v>
+      </c>
       <c r="P41" t="s">
-        <v>386</v>
+        <v>418</v>
       </c>
       <c r="Q41" t="s">
-        <v>387</v>
+        <v>419</v>
       </c>
       <c r="R41" t="s">
-        <v>388</v>
+        <v>420</v>
       </c>
       <c r="S41" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19">
+        <v>421</v>
+      </c>
+      <c r="T41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:50">
       <c r="A42">
         <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C42" t="s">
-        <v>390</v>
+        <v>422</v>
       </c>
       <c r="D42" t="s">
-        <v>391</v>
+        <v>423</v>
       </c>
       <c r="E42" t="s">
-        <v>392</v>
+        <v>424</v>
       </c>
       <c r="F42" t="s">
-        <v>393</v>
+        <v>425</v>
       </c>
       <c r="G42" t="s">
+        <v>54</v>
+      </c>
+      <c r="H42" t="s">
+        <v>426</v>
+      </c>
+      <c r="I42" t="s">
+        <v>422</v>
+      </c>
+      <c r="J42" t="s">
+        <v>424</v>
+      </c>
+      <c r="K42" t="s">
+        <v>425</v>
+      </c>
+      <c r="L42" t="s">
+        <v>52</v>
+      </c>
+      <c r="M42" t="s">
+        <v>427</v>
+      </c>
+      <c r="P42" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>429</v>
+      </c>
+      <c r="R42" t="s">
+        <v>430</v>
+      </c>
+      <c r="S42" t="s">
+        <v>424</v>
+      </c>
+      <c r="T42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:50">
+      <c r="A43">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
+        <v>431</v>
+      </c>
+      <c r="C43">
+        <v>9837635463</v>
+      </c>
+      <c r="D43" t="s">
+        <v>432</v>
+      </c>
+      <c r="E43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F43">
+        <v>2.592</v>
+      </c>
+      <c r="G43" t="s">
+        <v>27</v>
+      </c>
+      <c r="H43">
+        <v>7</v>
+      </c>
+      <c r="I43" t="s">
+        <v>171</v>
+      </c>
+      <c r="J43" t="s">
+        <v>172</v>
+      </c>
+      <c r="K43" t="s">
+        <v>433</v>
+      </c>
+      <c r="L43" t="s">
+        <v>173</v>
+      </c>
+      <c r="M43" t="s">
+        <v>434</v>
+      </c>
+      <c r="P43" t="s">
+        <v>435</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>435</v>
+      </c>
+      <c r="R43" t="s">
+        <v>420</v>
+      </c>
+      <c r="S43" t="s">
+        <v>436</v>
+      </c>
+      <c r="T43" t="s">
+        <v>437</v>
+      </c>
+      <c r="U43" t="s">
+        <v>438</v>
+      </c>
+      <c r="V43" t="s">
+        <v>439</v>
+      </c>
+      <c r="W43" t="s">
+        <v>440</v>
+      </c>
+      <c r="X43" t="s">
+        <v>441</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>441</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>443</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>444</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>445</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>444</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>446</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="44" spans="1:50">
+      <c r="A44">
+        <v>75</v>
+      </c>
+      <c r="B44" t="s">
+        <v>447</v>
+      </c>
+      <c r="C44">
+        <v>9843777683</v>
+      </c>
+      <c r="D44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M44" t="s">
+        <v>174</v>
+      </c>
+      <c r="P44" t="s">
+        <v>448</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>448</v>
+      </c>
+      <c r="T44" t="s">
+        <v>57</v>
+      </c>
+      <c r="U44" t="s">
+        <v>449</v>
+      </c>
+      <c r="V44" t="s">
+        <v>450</v>
+      </c>
+      <c r="W44" t="s">
+        <v>450</v>
+      </c>
+      <c r="X44" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>450</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>451</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>451</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>451</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>451</v>
+      </c>
+      <c r="AG44" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="45" spans="1:50">
+      <c r="A45">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45">
+        <v>9843777683</v>
+      </c>
+      <c r="D45" t="s">
+        <v>452</v>
+      </c>
+      <c r="E45" t="s">
+        <v>170</v>
+      </c>
+      <c r="F45">
+        <v>2.592</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>7</v>
+      </c>
+      <c r="I45" t="s">
+        <v>171</v>
+      </c>
+      <c r="J45" t="s">
+        <v>172</v>
+      </c>
+      <c r="K45" t="s">
+        <v>411</v>
+      </c>
+      <c r="L45" t="s">
+        <v>173</v>
+      </c>
+      <c r="M45" t="s">
+        <v>453</v>
+      </c>
+      <c r="P45" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>455</v>
+      </c>
+      <c r="R45" t="s">
+        <v>420</v>
+      </c>
+      <c r="S45" t="s">
+        <v>421</v>
+      </c>
+      <c r="T45" t="s">
+        <v>437</v>
+      </c>
+      <c r="U45" t="s">
+        <v>456</v>
+      </c>
+      <c r="V45" t="s">
+        <v>457</v>
+      </c>
+      <c r="W45" t="s">
+        <v>458</v>
+      </c>
+      <c r="X45" t="s">
+        <v>459</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>460</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>461</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>462</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>443</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>444</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>445</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>444</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>446</v>
+      </c>
+      <c r="AG45" t="s">
+        <v>444</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="46" spans="1:50">
+      <c r="A46">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>464</v>
+      </c>
+      <c r="C46">
+        <v>983436636</v>
+      </c>
+      <c r="D46" t="s">
+        <v>423</v>
+      </c>
+      <c r="E46" t="s">
+        <v>170</v>
+      </c>
+      <c r="F46">
+        <v>2.592</v>
+      </c>
+      <c r="G46" t="s">
+        <v>27</v>
+      </c>
+      <c r="H46">
+        <v>7</v>
+      </c>
+      <c r="I46" t="s">
+        <v>171</v>
+      </c>
+      <c r="J46" t="s">
+        <v>172</v>
+      </c>
+      <c r="K46" t="s">
+        <v>465</v>
+      </c>
+      <c r="L46" t="s">
+        <v>466</v>
+      </c>
+      <c r="M46" t="s">
+        <v>467</v>
+      </c>
+      <c r="P46" t="s">
+        <v>468</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>469</v>
+      </c>
+      <c r="R46" t="s">
+        <v>420</v>
+      </c>
+      <c r="S46" t="s">
+        <v>436</v>
+      </c>
+      <c r="T46" t="s">
+        <v>57</v>
+      </c>
+      <c r="U46" t="s">
+        <v>449</v>
+      </c>
+      <c r="V46">
+        <v>2036</v>
+      </c>
+      <c r="W46">
+        <v>2032</v>
+      </c>
+      <c r="X46">
+        <v>2030</v>
+      </c>
+      <c r="Y46">
+        <v>9</v>
+      </c>
+      <c r="Z46">
+        <v>3</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>470</v>
+      </c>
+      <c r="AB46">
+        <v>7</v>
+      </c>
+      <c r="AC46">
+        <v>7</v>
+      </c>
+      <c r="AD46">
+        <v>2</v>
+      </c>
+      <c r="AE46">
+        <v>9</v>
+      </c>
+      <c r="AF46">
+        <v>9</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>471</v>
+      </c>
+      <c r="AI46" t="s">
+        <v>472</v>
+      </c>
+      <c r="AK46" t="s">
+        <v>473</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>474</v>
+      </c>
+      <c r="AM46" t="s">
         <v>23</v>
       </c>
-      <c r="H42" t="s">
-        <v>394</v>
-      </c>
-      <c r="I42" t="s">
-        <v>390</v>
-      </c>
-      <c r="J42" t="s">
-        <v>392</v>
-      </c>
-      <c r="K42" t="s">
-        <v>393</v>
-      </c>
-      <c r="L42" t="s">
+      <c r="AN46" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO46">
+        <v>2038</v>
+      </c>
+      <c r="AP46">
+        <v>2.56</v>
+      </c>
+      <c r="AQ46">
+        <v>2.53</v>
+      </c>
+      <c r="AR46">
+        <v>2.54</v>
+      </c>
+      <c r="AS46">
+        <v>6</v>
+      </c>
+      <c r="AT46">
+        <v>9</v>
+      </c>
+      <c r="AU46">
+        <v>9</v>
+      </c>
+      <c r="AV46">
+        <v>9</v>
+      </c>
+      <c r="AW46">
+        <v>9</v>
+      </c>
+      <c r="AX46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:50">
+      <c r="A47">
+        <v>78</v>
+      </c>
+      <c r="B47" t="s">
+        <v>475</v>
+      </c>
+      <c r="C47">
+        <v>9834574657</v>
+      </c>
+      <c r="D47" t="s">
+        <v>476</v>
+      </c>
+      <c r="E47" t="s">
+        <v>477</v>
+      </c>
+      <c r="F47">
+        <v>3.5</v>
+      </c>
+      <c r="G47" t="s">
+        <v>27</v>
+      </c>
+      <c r="H47">
+        <v>7</v>
+      </c>
+      <c r="I47" t="s">
+        <v>478</v>
+      </c>
+      <c r="J47" t="s">
+        <v>479</v>
+      </c>
+      <c r="K47" t="s">
+        <v>480</v>
+      </c>
+      <c r="L47" t="s">
+        <v>481</v>
+      </c>
+      <c r="M47" t="s">
+        <v>482</v>
+      </c>
+      <c r="P47" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>484</v>
+      </c>
+      <c r="R47" t="s">
+        <v>436</v>
+      </c>
+      <c r="S47" t="s">
+        <v>485</v>
+      </c>
+      <c r="T47" t="s">
+        <v>57</v>
+      </c>
+      <c r="U47" t="s">
+        <v>486</v>
+      </c>
+      <c r="V47" t="s">
+        <v>487</v>
+      </c>
+      <c r="W47" t="s">
+        <v>474</v>
+      </c>
+      <c r="X47">
+        <v>2</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>488</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>462</v>
+      </c>
+      <c r="AB47">
+        <v>7</v>
+      </c>
+      <c r="AC47">
+        <v>6</v>
+      </c>
+      <c r="AD47">
+        <v>11</v>
+      </c>
+      <c r="AE47">
+        <v>2</v>
+      </c>
+      <c r="AF47">
+        <v>67</v>
+      </c>
+      <c r="AG47">
+        <v>114</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>489</v>
+      </c>
+      <c r="AK47">
+        <v>3.4</v>
+      </c>
+      <c r="AL47">
+        <v>2.5</v>
+      </c>
+      <c r="AM47">
+        <v>3.4</v>
+      </c>
+      <c r="AN47" t="s">
+        <v>490</v>
+      </c>
+      <c r="AO47">
+        <v>2080</v>
+      </c>
+      <c r="AP47">
+        <v>2077</v>
+      </c>
+      <c r="AQ47">
+        <v>2072</v>
+      </c>
+      <c r="AR47">
+        <v>2070</v>
+      </c>
+      <c r="AS47">
+        <v>7</v>
+      </c>
+      <c r="AT47">
+        <v>6</v>
+      </c>
+      <c r="AU47">
+        <v>11</v>
+      </c>
+      <c r="AV47">
+        <v>2</v>
+      </c>
+      <c r="AW47">
+        <v>76</v>
+      </c>
+      <c r="AX47">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:50">
+      <c r="A48">
+        <v>79</v>
+      </c>
+      <c r="B48" t="s">
+        <v>491</v>
+      </c>
+      <c r="C48">
+        <v>9834837444</v>
+      </c>
+      <c r="D48" t="s">
+        <v>492</v>
+      </c>
+      <c r="E48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F48">
+        <v>2.592</v>
+      </c>
+      <c r="G48" t="s">
+        <v>27</v>
+      </c>
+      <c r="H48">
         <v>21</v>
       </c>
-      <c r="M42" t="s">
-        <v>395</v>
-      </c>
-      <c r="N42"/>
-      <c r="O42"/>
-      <c r="P42" t="s">
-        <v>396</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>397</v>
-      </c>
-      <c r="R42" t="s">
-        <v>398</v>
-      </c>
-      <c r="S42" t="s">
-        <v>392</v>
+      <c r="I48" t="s">
+        <v>171</v>
+      </c>
+      <c r="J48" t="s">
+        <v>172</v>
+      </c>
+      <c r="K48" t="s">
+        <v>465</v>
+      </c>
+      <c r="L48" t="s">
+        <v>466</v>
+      </c>
+      <c r="M48" t="s">
+        <v>493</v>
+      </c>
+      <c r="P48" t="s">
+        <v>494</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>494</v>
+      </c>
+      <c r="R48" t="s">
+        <v>436</v>
+      </c>
+      <c r="S48" t="s">
+        <v>485</v>
+      </c>
+      <c r="T48" t="s">
+        <v>57</v>
+      </c>
+      <c r="U48" t="s">
+        <v>495</v>
+      </c>
+      <c r="V48" t="s">
+        <v>487</v>
+      </c>
+      <c r="W48" t="s">
+        <v>474</v>
+      </c>
+      <c r="X48">
+        <v>2</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>496</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>462</v>
+      </c>
+      <c r="AB48">
+        <v>7</v>
+      </c>
+      <c r="AC48">
+        <v>7</v>
+      </c>
+      <c r="AD48">
+        <v>2</v>
+      </c>
+      <c r="AE48">
+        <v>67</v>
+      </c>
+      <c r="AF48">
+        <v>7</v>
+      </c>
+      <c r="AG48">
+        <v>7</v>
+      </c>
+      <c r="AI48" t="s">
+        <v>472</v>
+      </c>
+      <c r="AK48">
+        <v>3.4</v>
+      </c>
+      <c r="AL48">
+        <v>2.578</v>
+      </c>
+      <c r="AM48">
+        <v>2.59</v>
+      </c>
+      <c r="AN48" t="s">
+        <v>477</v>
+      </c>
+      <c r="AO48">
+        <v>2080</v>
+      </c>
+      <c r="AP48">
+        <v>2077</v>
+      </c>
+      <c r="AQ48">
+        <v>2082</v>
+      </c>
+      <c r="AR48">
+        <v>2080</v>
+      </c>
+      <c r="AS48">
+        <v>6</v>
+      </c>
+      <c r="AT48">
+        <v>7</v>
+      </c>
+      <c r="AU48">
+        <v>7</v>
+      </c>
+      <c r="AV48">
+        <v>67</v>
+      </c>
+      <c r="AW48">
+        <v>77</v>
+      </c>
+      <c r="AX48">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:50">
+      <c r="A49">
+        <v>80</v>
+      </c>
+      <c r="P49" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>497</v>
+      </c>
+      <c r="T49" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ49" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="50" spans="1:50">
+      <c r="A50">
+        <v>81</v>
+      </c>
+      <c r="P50" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>499</v>
+      </c>
+      <c r="T50" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ50" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="51" spans="1:50">
+      <c r="A51">
+        <v>82</v>
+      </c>
+      <c r="B51" t="s">
+        <v>491</v>
+      </c>
+      <c r="M51" t="s">
+        <v>501</v>
+      </c>
+      <c r="P51" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>502</v>
+      </c>
+      <c r="T51" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ51" t="s">
+        <v>503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>